<commit_message>
altering tests to reflect name changes
</commit_message>
<xml_diff>
--- a/test/data/fake_samples_ENIGMA.xlsx
+++ b/test/data/fake_samples_ENIGMA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t xml:space="preserve">validation used:</t>
   </si>
@@ -37,9 +37,6 @@
     <t xml:space="preserve">user field</t>
   </si>
   <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
     <t xml:space="preserve">sampleid</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t xml:space="preserve">Jamboree</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">s1</t>
   </si>
   <si>
@@ -85,9 +79,6 @@
     <t xml:space="preserve">banjo</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">s2</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">fiddle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample 3</t>
   </si>
   <si>
     <t xml:space="preserve">s3</t>
@@ -231,42 +219,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -278,7 +266,7 @@
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -290,92 +278,80 @@
       <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="n">
+        <v>-50</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>-88</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>-50</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>-88</v>
-      </c>
-      <c r="H3" s="1" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="E5" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>-15</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>-15</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Id name changes (#52)
* switching to name as only required field, needs more edits

* altering tests to reflect name changes

* fixing up tests, waiting on appdev/ci to finish maintainence

* editing tests

* renaming id_field to name_field

* updating tests and fixing spots after merge

* fixing error file test by changing sample name col when populating errors

* changing 'id' fields to 'name' in ncbi uploader

* adding in logic for adding in node id in exporter

* iterating version
</commit_message>
<xml_diff>
--- a/test/data/fake_samples_ENIGMA.xlsx
+++ b/test/data/fake_samples_ENIGMA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t xml:space="preserve">validation used:</t>
   </si>
@@ -37,9 +37,6 @@
     <t xml:space="preserve">user field</t>
   </si>
   <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
     <t xml:space="preserve">sampleid</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t xml:space="preserve">Jamboree</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">s1</t>
   </si>
   <si>
@@ -85,9 +79,6 @@
     <t xml:space="preserve">banjo</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">s2</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">fiddle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample 3</t>
   </si>
   <si>
     <t xml:space="preserve">s3</t>
@@ -231,42 +219,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -278,7 +266,7 @@
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -290,92 +278,80 @@
       <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="n">
+        <v>-50</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>-88</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>-50</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>-88</v>
-      </c>
-      <c r="H3" s="1" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="E5" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>-15</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>-15</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>